<commit_message>
cleaning up the spreadsheets a little to try and help the parsing process
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/dnarepairmindataspreadsheets/Broad+others-DNA_repair.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/dnarepairmindataspreadsheets/Broad+others-DNA_repair.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="285">
   <si>
     <t>Instructions:
 Fill out from left to right.  Watch for red errors, correct them before moving on to the next column</t>
@@ -947,7 +947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -960,6 +960,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1419,11 +1422,7 @@
   <dimension ref="A1:BG51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2565" ySplit="7605" topLeftCell="A7931" activePane="topRight"/>
-      <selection activeCell="A52" sqref="A52:BG8101"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A3:A51"/>
-      <selection pane="bottomRight" activeCell="K7942" sqref="K7942"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1471,46 +1470,46 @@
       <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
       <c r="U1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="9"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="8" t="s">
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
     </row>
     <row r="2" spans="1:54" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1531,9 +1530,7 @@
       <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="G2" s="8"/>
       <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
@@ -4629,7 +4626,7 @@
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Z1:AB1"/>
   </mergeCells>
-  <dataValidations count="21">
+  <dataValidations disablePrompts="1" count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 I3 C3:C51">
       <formula1>biology</formula1>
     </dataValidation>
@@ -4695,7 +4692,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding a column header 'assay component role' for all the spreadsheet for cell 2/G
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/dnarepairmindataspreadsheets/Broad+others-DNA_repair.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/dnarepairmindataspreadsheets/Broad+others-DNA_repair.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="286">
   <si>
     <t>Instructions:
 Fill out from left to right.  Watch for red errors, correct them before moving on to the next column</t>
@@ -897,6 +897,9 @@
   </si>
   <si>
     <t>540 nm</t>
+  </si>
+  <si>
+    <t>assay component role</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1533,9 @@
       <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
@@ -4626,7 +4631,7 @@
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Z1:AB1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="21">
+  <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 I3 C3:C51">
       <formula1>biology</formula1>
     </dataValidation>

</xml_diff>